<commit_message>
Verify case sensitivity in password
</commit_message>
<xml_diff>
--- a/Test Data/ECT-TestCases.xlsx
+++ b/Test Data/ECT-TestCases.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="121">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -485,6 +485,27 @@
   </si>
   <si>
     <t>TC-SIGNIN-010</t>
+  </si>
+  <si>
+    <t>Verify password case sensitivity</t>
+  </si>
+  <si>
+    <t>Test signing in with passwords that differ in case</t>
+  </si>
+  <si>
+    <t>1. Navigate to 'sign in' page
+2.Enter Email Address into email address field.
+3.Enter Password  that has different letter cases.
+4.Click on 'sign in' button</t>
+  </si>
+  <si>
+    <t>{
+        "Email": "yadvirkaur@mailinator.com",
+        "Password": "YaDvIr@001"
+    }</t>
+  </si>
+  <si>
+    <t>Sign-in should fail if the password is case-sensitive.</t>
   </si>
 </sst>
 </file>
@@ -1131,7 +1152,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1158,6 +1179,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1774,7 +1798,7 @@
       <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1803,7 +1827,7 @@
       <c r="H3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1832,7 +1856,7 @@
       <c r="H4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1861,7 +1885,7 @@
       <c r="H5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1887,7 +1911,7 @@
       <c r="H6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1913,7 +1937,7 @@
       <c r="H7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1939,7 +1963,7 @@
       <c r="H8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1954,8 +1978,8 @@
   <sheetPr/>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -2025,7 +2049,7 @@
       <c r="H2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="10" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2054,7 +2078,7 @@
       <c r="H3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="11" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2083,7 +2107,7 @@
       <c r="H4" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="11" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2112,7 +2136,7 @@
       <c r="H5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="11" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2138,7 +2162,7 @@
       <c r="G6" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="11" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2167,7 +2191,7 @@
       <c r="H7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="11" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2196,7 +2220,7 @@
       <c r="H8" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="11" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2222,7 +2246,7 @@
       <c r="H9" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="11" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2252,9 +2276,27 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" ht="16.2" spans="1:1">
+    <row r="11" ht="97.2" spans="1:7">
       <c r="A11" s="3" t="s">
         <v>115</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Verify Forgot Password Link Navigation
</commit_message>
<xml_diff>
--- a/Test Data/ECT-TestCases.xlsx
+++ b/Test Data/ECT-TestCases.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="127">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -506,6 +506,27 @@
   </si>
   <si>
     <t>Sign-in should fail if the password is case-sensitive.</t>
+  </si>
+  <si>
+    <t>TC-SIGNIN-011</t>
+  </si>
+  <si>
+    <t>Verify Forgot Password Link Navigation</t>
+  </si>
+  <si>
+    <t>To verify that clicking the "Forgot Your Password?" link on the Sign-In page redirects the user to the correct "Forgot Password" page.</t>
+  </si>
+  <si>
+    <t>1. Navigate to 'sign in' page
+2. Locate and click on the "Forgot Your Password?" link.
+3. Wait for the page to load.
+4. Verify the URL and the page title.</t>
+  </si>
+  <si>
+    <t>User should be redirected to the "Forgot Password" page. The URL should match the "Forgot Password" page endpoint, and the page title should confirm the navigation.</t>
+  </si>
+  <si>
+    <t>User is redirected to the "Forgot Password" page and the page title is confirm the navigation.</t>
   </si>
 </sst>
 </file>
@@ -1158,7 +1179,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1182,6 +1203,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1804,7 +1831,7 @@
       <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1833,7 +1860,7 @@
       <c r="H3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1862,7 +1889,7 @@
       <c r="H4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1891,7 +1918,7 @@
       <c r="H5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1917,7 +1944,7 @@
       <c r="H6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1943,7 +1970,7 @@
       <c r="H7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1969,7 +1996,7 @@
       <c r="H8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1982,10 +2009,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -2055,7 +2082,7 @@
       <c r="H2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="11" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2084,7 +2111,7 @@
       <c r="H3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="12" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2113,7 +2140,7 @@
       <c r="H4" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2142,7 +2169,7 @@
       <c r="H5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2168,7 +2195,7 @@
       <c r="G6" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2197,7 +2224,7 @@
       <c r="H7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2226,7 +2253,7 @@
       <c r="H8" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2252,7 +2279,7 @@
       <c r="H9" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2281,7 +2308,7 @@
       <c r="H10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="13" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2311,6 +2338,35 @@
         <v>73</v>
       </c>
       <c r="I11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" ht="162" spans="1:9">
+      <c r="A12" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I12" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Verify error message for invalid email
</commit_message>
<xml_diff>
--- a/Test Data/ECT-TestCases.xlsx
+++ b/Test Data/ECT-TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="10440" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp_Tests" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="140">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -552,7 +552,35 @@
   <si>
     <t>{
         "Email": "navjotsingh@mailinator.com",
+       "Password":
+          "Navjot@001",
+"ConfirmPassword":
+"Navjot@001"
     }</t>
+  </si>
+  <si>
+    <t>FP-003</t>
+  </si>
+  <si>
+    <t>Verify error message for invalid email</t>
+  </si>
+  <si>
+    <t>To ensure that an appropriate error message is displayed for invalid email formats.</t>
+  </si>
+  <si>
+    <t>1. Navigate to 'sign in' page
+2.Navigate to 'Forgot Password' page.
+3.Enter an invalid email format 
+3. Click the submit button.
+4. Verify the displayed error message.</t>
+  </si>
+  <si>
+    <t>{
+        "Email": "navjotsingh.com"
+    }</t>
+  </si>
+  <si>
+    <t>An error message  should be displayed.</t>
   </si>
 </sst>
 </file>
@@ -1233,14 +1261,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1839,7 +1867,7 @@
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -1848,16 +1876,16 @@
       <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="I2" s="15" t="s">
@@ -1868,7 +1896,7 @@
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -1877,16 +1905,16 @@
       <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="11" t="s">
         <v>22</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I3" s="15" t="s">
@@ -1897,25 +1925,25 @@
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="4" t="s">
         <v>31</v>
       </c>
       <c r="I4" s="15" t="s">
@@ -1926,25 +1954,25 @@
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="4" t="s">
         <v>38</v>
       </c>
       <c r="I5" s="15" t="s">
@@ -1955,22 +1983,22 @@
       <c r="A6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="4" t="s">
         <v>44</v>
       </c>
       <c r="I6" s="15" t="s">
@@ -1981,22 +2009,22 @@
       <c r="A7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="4" t="s">
         <v>51</v>
       </c>
       <c r="I7" s="15" t="s">
@@ -2007,22 +2035,22 @@
       <c r="A8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="4" t="s">
         <v>57</v>
       </c>
       <c r="I8" s="15" t="s">
@@ -2090,7 +2118,7 @@
       <c r="A2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -2099,16 +2127,16 @@
       <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>63</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="4" t="s">
         <v>65</v>
       </c>
       <c r="I2" s="12" t="s">
@@ -2119,7 +2147,7 @@
       <c r="A3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -2128,10 +2156,10 @@
       <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="4" t="s">
         <v>71</v>
       </c>
       <c r="G3" s="5" t="s">
@@ -2148,7 +2176,7 @@
       <c r="A4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -2157,10 +2185,10 @@
       <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="4" t="s">
         <v>79</v>
       </c>
       <c r="G4" s="5" t="s">
@@ -2177,25 +2205,25 @@
       <c r="A5" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="4" t="s">
         <v>81</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="4" t="s">
         <v>44</v>
       </c>
       <c r="I5" s="13" t="s">
@@ -2206,7 +2234,7 @@
       <c r="A6" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="4" t="s">
         <v>85</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -2215,10 +2243,10 @@
       <c r="D6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="4" t="s">
         <v>89</v>
       </c>
       <c r="G6" s="5" t="s">
@@ -2232,25 +2260,25 @@
       <c r="A7" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="4" t="s">
         <v>57</v>
       </c>
       <c r="I7" s="13" t="s">
@@ -2261,25 +2289,25 @@
       <c r="A8" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="4" t="s">
         <v>99</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="4" t="s">
         <v>103</v>
       </c>
       <c r="I8" s="13" t="s">
@@ -2290,22 +2318,22 @@
       <c r="A9" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="4" t="s">
         <v>106</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="4" t="s">
         <v>109</v>
       </c>
       <c r="I9" s="13" t="s">
@@ -2316,25 +2344,25 @@
       <c r="A10" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="4" t="s">
         <v>112</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="11" t="s">
         <v>114</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="4" t="s">
         <v>65</v>
       </c>
       <c r="I10" s="14" t="s">
@@ -2345,22 +2373,22 @@
       <c r="A11" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="4" t="s">
         <v>117</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="4" t="s">
         <v>120</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -2414,13 +2442,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="34.5555555555556" customWidth="1"/>
@@ -2485,13 +2513,42 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" ht="72" spans="1:6">
+    <row r="3" ht="115.2" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>132</v>
       </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="F3" s="7" t="s">
         <v>133</v>
       </c>
+    </row>
+    <row r="4" ht="81" spans="1:7">
+      <c r="A4" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="7:7">
+      <c r="G5" s="9"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Verify error message for empty email field
</commit_message>
<xml_diff>
--- a/Test Data/ECT-TestCases.xlsx
+++ b/Test Data/ECT-TestCases.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="149">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -547,6 +547,9 @@
     <t>Email input field should be present.</t>
   </si>
   <si>
+    <t>Email input field is present on the forgot password page.</t>
+  </si>
+  <si>
     <t>FP-002</t>
   </si>
   <si>
@@ -580,7 +583,37 @@
     }</t>
   </si>
   <si>
+    <t>An error message  should be displayed  for invalid email format.</t>
+  </si>
+  <si>
+    <t>An error message is displayed for invalid email format as expected.</t>
+  </si>
+  <si>
+    <t>FP-004</t>
+  </si>
+  <si>
+    <t>Verify error message for empty email field</t>
+  </si>
+  <si>
+    <t>To ensure that an error message is displayed if the email field is left empty.</t>
+  </si>
+  <si>
+    <t>1. Navigate to 'sign in' page
+2.Navigate to 'Forgot Password' page.
+3.Don't enter anything in email address field. 
+3. Click the submit button.
+4. Verify the displayed error message.</t>
+  </si>
+  <si>
+    <t>{
+        "Email": ""
+    }</t>
+  </si>
+  <si>
     <t>An error message  should be displayed.</t>
+  </si>
+  <si>
+    <t>An error message is displayed for empty email address field as expected.</t>
   </si>
 </sst>
 </file>
@@ -1233,7 +1266,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1255,13 +1288,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1876,10 +1903,10 @@
       <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="9" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="5" t="s">
@@ -1888,7 +1915,7 @@
       <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="13" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1905,10 +1932,10 @@
       <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>22</v>
       </c>
       <c r="G3" s="5" t="s">
@@ -1917,7 +1944,7 @@
       <c r="H3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="13" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1937,7 +1964,7 @@
       <c r="E4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="9" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -1946,7 +1973,7 @@
       <c r="H4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="13" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1966,7 +1993,7 @@
       <c r="E5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="9" t="s">
         <v>36</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -1975,7 +2002,7 @@
       <c r="H5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="13" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2001,7 +2028,7 @@
       <c r="H6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="13" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2027,7 +2054,7 @@
       <c r="H7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="13" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2053,7 +2080,7 @@
       <c r="H8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="13" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2127,10 +2154,10 @@
       <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="9" t="s">
         <v>63</v>
       </c>
       <c r="G2" s="5" t="s">
@@ -2139,7 +2166,7 @@
       <c r="H2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2156,7 +2183,7 @@
       <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="8" t="s">
         <v>70</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -2168,7 +2195,7 @@
       <c r="H3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="11" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2185,7 +2212,7 @@
       <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>78</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -2197,7 +2224,7 @@
       <c r="H4" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="11" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2226,7 +2253,7 @@
       <c r="H5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="11" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2243,7 +2270,7 @@
       <c r="D6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>88</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -2252,7 +2279,7 @@
       <c r="G6" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="11" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2281,7 +2308,7 @@
       <c r="H7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="11" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2310,7 +2337,7 @@
       <c r="H8" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="11" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2336,7 +2363,7 @@
       <c r="H9" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="11" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2353,10 +2380,10 @@
       <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="9" t="s">
         <v>114</v>
       </c>
       <c r="G10" s="5" t="s">
@@ -2365,7 +2392,7 @@
       <c r="H10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2382,7 +2409,7 @@
       <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="8" t="s">
         <v>118</v>
       </c>
       <c r="F11" s="4" t="s">
@@ -2445,7 +2472,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4"/>
@@ -2490,7 +2517,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" ht="64.8" spans="1:7">
+    <row r="2" ht="64.8" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>127</v>
       </c>
@@ -2512,43 +2539,72 @@
       <c r="G2" s="4" t="s">
         <v>131</v>
       </c>
+      <c r="H2" s="4" t="s">
+        <v>132</v>
+      </c>
     </row>
-    <row r="3" ht="115.2" spans="1:6">
+    <row r="3" ht="145.8" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>133</v>
+      <c r="F3" s="4" t="s">
+        <v>134</v>
       </c>
     </row>
-    <row r="4" ht="81" spans="1:7">
+    <row r="4" ht="81" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B4" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>136</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="G4" s="8" t="s">
         <v>139</v>
       </c>
+      <c r="G4" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>141</v>
+      </c>
     </row>
-    <row r="5" spans="7:7">
-      <c r="G5" s="9"/>
+    <row r="5" ht="97.2" spans="1:8">
+      <c r="A5" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
verify forgot password functionality with valid email address
</commit_message>
<xml_diff>
--- a/Test Data/ECT-TestCases.xlsx
+++ b/Test Data/ECT-TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9995" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp_Tests" sheetId="1" r:id="rId1"/>
@@ -2095,8 +2095,8 @@
   <sheetPr/>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -2471,8 +2471,8 @@
   <sheetPr/>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I$1:I$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4"/>

</xml_diff>

<commit_message>
Verify sign in after resetting password
</commit_message>
<xml_diff>
--- a/Test Data/ECT-TestCases.xlsx
+++ b/Test Data/ECT-TestCases.xlsx
@@ -547,7 +547,9 @@
   <si>
     <t>{
         "Email": "navjotsingh@mailinator.com",
-        "Password": "Navjot@001"
+        "Password": "Navjot@001",
+"FirstName": "Navjot",
+        "LastName": "Singh"
     }</t>
   </si>
   <si>
@@ -2165,8 +2167,8 @@
   <sheetPr/>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:H13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -2524,7 +2526,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" ht="81" spans="1:9">
+    <row r="13" ht="113.4" spans="1:9">
       <c r="A13" s="3" t="s">
         <v>127</v>
       </c>

</xml_diff>

<commit_message>
Verify search field visibility and type
</commit_message>
<xml_diff>
--- a/Test Data/ECT-TestCases.xlsx
+++ b/Test Data/ECT-TestCases.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="181">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -714,6 +714,27 @@
   <si>
     <t>1. The logo is visible on the homepage.
 2. Clicking the logo successfully navigates the user back to the homepage.</t>
+  </si>
+  <si>
+    <t>HP-002</t>
+  </si>
+  <si>
+    <t>Verify search field visibility and type</t>
+  </si>
+  <si>
+    <t>Ensure the search field is visible on the page and is of type input to accept user input.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the Home page.
+2. Locate the search field.
+3. Check if the search field is visible.
+4. Verify the type of the search field is "input".</t>
+  </si>
+  <si>
+    <t>The search field should be visible on the page, and the element type should be "input".</t>
+  </si>
+  <si>
+    <t>Search field is visible and confirmed as input.</t>
   </si>
 </sst>
 </file>
@@ -2815,13 +2836,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="22.4444444444444" customWidth="1"/>
     <col min="2" max="2" width="35.7777777777778" customWidth="1"/>
@@ -2888,11 +2909,39 @@
       <c r="H2" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="I2" s="6"/>
+      <c r="I2" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" ht="97.2" spans="1:8">
+      <c r="A3" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>180</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I$1:I$1048576">
       <formula1>"Passed,Failed,In Progress"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Cart button should be visible and clickable
</commit_message>
<xml_diff>
--- a/Test Data/ECT-TestCases.xlsx
+++ b/Test Data/ECT-TestCases.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="181">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -722,19 +722,19 @@
     <t>Verify search field visibility and type</t>
   </si>
   <si>
-    <t>Ensure the search field is visible on the page and is of type input to accept user input.</t>
-  </si>
-  <si>
-    <t>1. Navigate to the Home page.
-2. Locate the search field.
-3. Check if the search field is visible.
-4. Verify the type of the search field is "input".</t>
-  </si>
-  <si>
-    <t>The search field should be visible on the page, and the element type should be "input".</t>
-  </si>
-  <si>
-    <t>Search field is visible and confirmed as input.</t>
+    <t>Ensure the search field is accessible and functional, allowing users to input search queries.</t>
+  </si>
+  <si>
+    <t>1. Open the homepage.
+2. Locate the logo element on the homepage.
+3. Ensure the search field is visible.
+4. Check the input type attribute of the field (i.e., text).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The search field should be  visible and should accept text input. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The search field is visible and accepts text input. </t>
   </si>
 </sst>
 </file>
@@ -1413,11 +1413,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2025,7 +2025,7 @@
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -2043,7 +2043,7 @@
       <c r="G2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="I2" s="14" t="s">
@@ -2054,7 +2054,7 @@
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -2072,7 +2072,7 @@
       <c r="G3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I3" s="14" t="s">
@@ -2083,25 +2083,25 @@
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>28</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="4" t="s">
         <v>31</v>
       </c>
       <c r="I4" s="14" t="s">
@@ -2112,25 +2112,25 @@
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="4" t="s">
         <v>38</v>
       </c>
       <c r="I5" s="14" t="s">
@@ -2141,22 +2141,22 @@
       <c r="A6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="4" t="s">
         <v>44</v>
       </c>
       <c r="I6" s="14" t="s">
@@ -2167,22 +2167,22 @@
       <c r="A7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="4" t="s">
         <v>51</v>
       </c>
       <c r="I7" s="14" t="s">
@@ -2193,22 +2193,22 @@
       <c r="A8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="4" t="s">
         <v>57</v>
       </c>
       <c r="I8" s="14" t="s">
@@ -2226,7 +2226,7 @@
   <sheetPr/>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -2276,7 +2276,7 @@
       <c r="A2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -2294,7 +2294,7 @@
       <c r="G2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="4" t="s">
         <v>65</v>
       </c>
       <c r="I2" s="11" t="s">
@@ -2305,7 +2305,7 @@
       <c r="A3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -2317,7 +2317,7 @@
       <c r="E3" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="4" t="s">
         <v>71</v>
       </c>
       <c r="G3" s="5" t="s">
@@ -2334,7 +2334,7 @@
       <c r="A4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -2346,7 +2346,7 @@
       <c r="E4" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="4" t="s">
         <v>79</v>
       </c>
       <c r="G4" s="5" t="s">
@@ -2363,25 +2363,25 @@
       <c r="A5" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>81</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="4" t="s">
         <v>44</v>
       </c>
       <c r="I5" s="12" t="s">
@@ -2392,7 +2392,7 @@
       <c r="A6" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>85</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -2404,7 +2404,7 @@
       <c r="E6" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="4" t="s">
         <v>89</v>
       </c>
       <c r="G6" s="5" t="s">
@@ -2418,25 +2418,25 @@
       <c r="A7" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="4" t="s">
         <v>57</v>
       </c>
       <c r="I7" s="12" t="s">
@@ -2447,25 +2447,25 @@
       <c r="A8" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>99</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="4" t="s">
         <v>100</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="4" t="s">
         <v>103</v>
       </c>
       <c r="I8" s="12" t="s">
@@ -2476,22 +2476,22 @@
       <c r="A9" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="4" t="s">
         <v>106</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="4" t="s">
         <v>109</v>
       </c>
       <c r="I9" s="12" t="s">
@@ -2502,10 +2502,10 @@
       <c r="A10" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="4" t="s">
         <v>112</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -2520,7 +2520,7 @@
       <c r="G10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="4" t="s">
         <v>65</v>
       </c>
       <c r="I10" s="13" t="s">
@@ -2531,10 +2531,10 @@
       <c r="A11" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="4" t="s">
         <v>117</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -2543,10 +2543,10 @@
       <c r="E11" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="4" t="s">
         <v>120</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -2560,25 +2560,25 @@
       <c r="A12" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="4" t="s">
         <v>123</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="4" t="s">
         <v>124</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="4" t="s">
         <v>126</v>
       </c>
       <c r="I12" t="s">
@@ -2601,7 +2601,7 @@
       <c r="E13" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="4" t="s">
         <v>131</v>
       </c>
       <c r="G13" s="4" t="s">
@@ -2681,25 +2681,25 @@
       <c r="A2" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>136</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>137</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="4" t="s">
         <v>139</v>
       </c>
       <c r="I2" t="s">
@@ -2710,25 +2710,25 @@
       <c r="A3" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>142</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="4" t="s">
         <v>146</v>
       </c>
       <c r="I3" t="s">
@@ -2739,25 +2739,25 @@
       <c r="A4" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>149</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="4" t="s">
         <v>153</v>
       </c>
       <c r="I4" t="s">
@@ -2768,25 +2768,25 @@
       <c r="A5" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>156</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="4" t="s">
         <v>160</v>
       </c>
       <c r="I5" t="s">
@@ -2797,25 +2797,25 @@
       <c r="A6" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="4" t="s">
         <v>163</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="4" t="s">
         <v>167</v>
       </c>
       <c r="I6" t="s">
@@ -2838,8 +2838,8 @@
   <sheetPr/>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
@@ -2909,34 +2909,37 @@
       <c r="H2" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" ht="97.2" spans="1:8">
+    <row r="3" ht="113.4" spans="1:9">
       <c r="A3" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>177</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6" t="s">
         <v>178</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="6" t="s">
         <v>180</v>
+      </c>
+      <c r="I3" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Verify Add to Wishlist Functionality After Login
</commit_message>
<xml_diff>
--- a/Test Data/ECT-TestCases.xlsx
+++ b/Test Data/ECT-TestCases.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="256">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -994,6 +994,34 @@
   </si>
   <si>
     <t>Verify Add to Wishlist Functionality After Login</t>
+  </si>
+  <si>
+    <t>Ensure that clicking on the "Add to Wishlist" icon after logging in navigates the user to the wishlist page and displays a success message.</t>
+  </si>
+  <si>
+    <t>1. Log in to the application with valid credentials.
+2. Navigate to the home page.
+3. Hover over a product image in the Hot Sellers section.
+4. Verify the "Add to Wishlist" icon is visible.
+5. Click on the "Add to Wishlist" icon.
+6. Verify that the user is navigated to the wishlist page.
+7. Verify that a success message is displayed confirming the item was added to the wishlist.</t>
+  </si>
+  <si>
+    <t>{
+        "Email": "navjotsingh@mailinator.com",
+        "Password": "Navjot@001"
+}</t>
+  </si>
+  <si>
+    <t>1. "Add to Wishlist" icon is visible upon hovering.
+2. Clicking the icon navigates the user to the wishlist page.
+3. A success message appears confirming the item was added to the wishlist.</t>
+  </si>
+  <si>
+    <t>1. "Add to Wishlist" icon was visible upon hovering.
+2. Clicking the icon successfully navigated the user to the wishlist page.
+3. A success message, "Item added to your wishlist," was displayed.</t>
   </si>
 </sst>
 </file>
@@ -1653,7 +1681,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1673,9 +1701,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -2296,10 +2321,10 @@
       <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="5" t="s">
@@ -2308,7 +2333,7 @@
       <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2325,10 +2350,10 @@
       <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G3" s="5" t="s">
@@ -2337,7 +2362,7 @@
       <c r="H3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2357,7 +2382,7 @@
       <c r="E4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -2366,7 +2391,7 @@
       <c r="H4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2386,7 +2411,7 @@
       <c r="E5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="10" t="s">
         <v>36</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -2395,7 +2420,7 @@
       <c r="H5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2421,7 +2446,7 @@
       <c r="H6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2447,7 +2472,7 @@
       <c r="H7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2473,7 +2498,7 @@
       <c r="H8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2489,7 +2514,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:B14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -2547,10 +2572,10 @@
       <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>63</v>
       </c>
       <c r="G2" s="5" t="s">
@@ -2559,7 +2584,7 @@
       <c r="H2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2576,7 +2601,7 @@
       <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>70</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -2588,7 +2613,7 @@
       <c r="H3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="12" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2605,7 +2630,7 @@
       <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>78</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -2617,7 +2642,7 @@
       <c r="H4" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2646,7 +2671,7 @@
       <c r="H5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2663,7 +2688,7 @@
       <c r="D6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>88</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -2672,7 +2697,7 @@
       <c r="G6" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2701,7 +2726,7 @@
       <c r="H7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2721,7 +2746,7 @@
       <c r="E8" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>101</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -2730,7 +2755,7 @@
       <c r="H8" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2756,7 +2781,7 @@
       <c r="H9" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2773,10 +2798,10 @@
       <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>114</v>
       </c>
       <c r="G10" s="5" t="s">
@@ -2785,7 +2810,7 @@
       <c r="H10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="13" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2802,7 +2827,7 @@
       <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>118</v>
       </c>
       <c r="F11" s="4" t="s">
@@ -2834,7 +2859,7 @@
       <c r="E12" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="8" t="s">
         <v>101</v>
       </c>
       <c r="G12" s="4" t="s">
@@ -2860,7 +2885,7 @@
       <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>130</v>
       </c>
       <c r="F13" s="4" t="s">
@@ -2955,7 +2980,7 @@
       <c r="E2" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>101</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -3100,8 +3125,8 @@
   <sheetPr/>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -3171,7 +3196,7 @@
       <c r="H2" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3552,14 +3577,34 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" ht="28.8" spans="1:3">
+    <row r="16" ht="226.8" spans="1:9">
       <c r="A16" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="C16" s="7"/>
+      <c r="C16" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="I16" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Verify Visibility and Navigation of Reviews with Star Rating under Hot Sellers Image
</commit_message>
<xml_diff>
--- a/Test Data/ECT-TestCases.xlsx
+++ b/Test Data/ECT-TestCases.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="262">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -1046,7 +1046,7 @@
   </si>
   <si>
     <t>1. Star ratings and reviews were visible under the product image.
-2. Clicking the reviews link navigated the user to the product's review section</t>
+2. Clicking the reviews link successfully navigated the user to the product's review section</t>
   </si>
 </sst>
 </file>
@@ -1706,7 +1706,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1726,9 +1726,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -2349,10 +2346,10 @@
       <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="5" t="s">
@@ -2361,7 +2358,7 @@
       <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2378,10 +2375,10 @@
       <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G3" s="5" t="s">
@@ -2390,7 +2387,7 @@
       <c r="H3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2410,7 +2407,7 @@
       <c r="E4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -2419,7 +2416,7 @@
       <c r="H4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2439,7 +2436,7 @@
       <c r="E5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="10" t="s">
         <v>36</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -2448,7 +2445,7 @@
       <c r="H5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2474,7 +2471,7 @@
       <c r="H6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2500,7 +2497,7 @@
       <c r="H7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2526,7 +2523,7 @@
       <c r="H8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2600,10 +2597,10 @@
       <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>63</v>
       </c>
       <c r="G2" s="5" t="s">
@@ -2612,7 +2609,7 @@
       <c r="H2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2629,7 +2626,7 @@
       <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>70</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -2641,7 +2638,7 @@
       <c r="H3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="12" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2658,7 +2655,7 @@
       <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>78</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -2670,7 +2667,7 @@
       <c r="H4" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2699,7 +2696,7 @@
       <c r="H5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2716,7 +2713,7 @@
       <c r="D6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>88</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -2725,7 +2722,7 @@
       <c r="G6" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2754,7 +2751,7 @@
       <c r="H7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2774,7 +2771,7 @@
       <c r="E8" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>101</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -2783,7 +2780,7 @@
       <c r="H8" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2809,7 +2806,7 @@
       <c r="H9" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2826,10 +2823,10 @@
       <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>114</v>
       </c>
       <c r="G10" s="5" t="s">
@@ -2838,7 +2835,7 @@
       <c r="H10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="13" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2855,7 +2852,7 @@
       <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>118</v>
       </c>
       <c r="F11" s="4" t="s">
@@ -2887,7 +2884,7 @@
       <c r="E12" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="8" t="s">
         <v>101</v>
       </c>
       <c r="G12" s="4" t="s">
@@ -2913,7 +2910,7 @@
       <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>130</v>
       </c>
       <c r="F13" s="4" t="s">
@@ -3008,7 +3005,7 @@
       <c r="E2" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>101</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -3153,8 +3150,8 @@
   <sheetPr/>
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D15" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -3224,7 +3221,7 @@
       <c r="H2" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3634,30 +3631,33 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" ht="129.6" spans="1:8">
+    <row r="17" ht="194.4" spans="1:9">
       <c r="A17" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>258</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>259</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="6" t="s">
         <v>261</v>
+      </c>
+      <c r="I17" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Verify "Add to Cart" Button and Product Options on Product Page
</commit_message>
<xml_diff>
--- a/Test Data/ECT-TestCases.xlsx
+++ b/Test Data/ECT-TestCases.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="274">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -1075,6 +1075,9 @@
     <t>The product page should load with the correct product details and display a visible "Add to Cart" button with options.</t>
   </si>
   <si>
+    <t>PP-002</t>
+  </si>
+  <si>
     <t>Verify the visibility and functionality of the quantity field on the product page</t>
   </si>
   <si>
@@ -1084,7 +1087,11 @@
     <t xml:space="preserve">1. Open the home page.
 2. Locate and click on a product image.
 3. Locate the quantity field on product page.
+4. Verify it is visible and input type.
 </t>
+  </si>
+  <si>
+    <t>The quantity field should be visible, input-enabled, and functional. Users should be able to adjust the quantity.</t>
   </si>
 </sst>
 </file>
@@ -1113,13 +1120,13 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF091E42"/>
+      <color theme="1"/>
       <name val="Verdana"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF091E42"/>
       <name val="Verdana"/>
       <charset val="134"/>
     </font>
@@ -1744,7 +1751,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1752,6 +1759,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1760,28 +1779,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2372,196 +2385,196 @@
       </c>
     </row>
     <row r="2" ht="162" spans="1:9">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" ht="129.6" spans="1:9">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" ht="129.6" spans="1:9">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" ht="129.6" spans="1:9">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" ht="81" spans="1:9">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" ht="145.8" spans="1:9">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" ht="194.4" spans="1:9">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="16" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2623,283 +2636,283 @@
       </c>
     </row>
     <row r="2" ht="113.4" spans="1:9">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="13" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3" ht="81" spans="1:9">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="14" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="4" ht="81" spans="1:9">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="14" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" ht="113.4" spans="1:9">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="14" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" ht="97.2" spans="1:9">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="14" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="7" ht="194.4" spans="1:9">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="14" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="8" ht="129.6" spans="1:9">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="14" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="9" ht="178.2" spans="1:9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="14" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="10" ht="113.4" spans="1:9">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="11" ht="97.2" spans="1:9">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="5" t="s">
         <v>73</v>
       </c>
       <c r="I11" t="s">
@@ -2907,28 +2920,28 @@
       </c>
     </row>
     <row r="12" ht="162" spans="1:9">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="8" t="s">
         <v>126</v>
       </c>
       <c r="I12" t="s">
@@ -2936,28 +2949,28 @@
       </c>
     </row>
     <row r="13" ht="113.4" spans="1:9">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="8" t="s">
         <v>133</v>
       </c>
       <c r="I13" t="s">
@@ -3028,28 +3041,28 @@
       </c>
     </row>
     <row r="2" ht="64.8" spans="1:9">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="8" t="s">
         <v>139</v>
       </c>
       <c r="I2" t="s">
@@ -3057,28 +3070,28 @@
       </c>
     </row>
     <row r="3" ht="129.6" spans="1:9">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="8" t="s">
         <v>146</v>
       </c>
       <c r="I3" t="s">
@@ -3086,28 +3099,28 @@
       </c>
     </row>
     <row r="4" ht="97.2" spans="1:9">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="8" t="s">
         <v>153</v>
       </c>
       <c r="I4" t="s">
@@ -3115,28 +3128,28 @@
       </c>
     </row>
     <row r="5" ht="113.4" spans="1:9">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="8" t="s">
         <v>160</v>
       </c>
       <c r="I5" t="s">
@@ -3144,28 +3157,28 @@
       </c>
     </row>
     <row r="6" ht="113.4" spans="1:9">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="8" t="s">
         <v>167</v>
       </c>
       <c r="I6" t="s">
@@ -3188,8 +3201,8 @@
   <sheetPr/>
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -3235,57 +3248,57 @@
       </c>
     </row>
     <row r="2" ht="145.8" spans="1:9">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3" ht="113.4" spans="1:9">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="8" t="s">
         <v>180</v>
       </c>
       <c r="I3" t="s">
@@ -3293,28 +3306,28 @@
       </c>
     </row>
     <row r="4" ht="97.2" spans="1:9">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="8" t="s">
         <v>186</v>
       </c>
       <c r="I4" t="s">
@@ -3322,28 +3335,28 @@
       </c>
     </row>
     <row r="5" ht="97.2" spans="1:9">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="8" t="s">
         <v>192</v>
       </c>
       <c r="I5" t="s">
@@ -3351,28 +3364,28 @@
       </c>
     </row>
     <row r="6" ht="129.6" spans="1:9">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="8" t="s">
         <v>198</v>
       </c>
       <c r="I6" t="s">
@@ -3380,28 +3393,28 @@
       </c>
     </row>
     <row r="7" ht="129.6" spans="1:9">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="8" t="s">
         <v>204</v>
       </c>
       <c r="I7" t="s">
@@ -3409,28 +3422,28 @@
       </c>
     </row>
     <row r="8" ht="210.6" spans="1:9">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I8" t="s">
@@ -3438,28 +3451,28 @@
       </c>
     </row>
     <row r="9" ht="210.6" spans="1:9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="8" t="s">
         <v>216</v>
       </c>
       <c r="I9" t="s">
@@ -3467,28 +3480,28 @@
       </c>
     </row>
     <row r="10" ht="226.8" spans="1:9">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I10" t="s">
@@ -3496,28 +3509,28 @@
       </c>
     </row>
     <row r="11" ht="226.8" spans="1:9">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I11" t="s">
@@ -3525,28 +3538,28 @@
       </c>
     </row>
     <row r="12" ht="129.6" spans="1:9">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="8" t="s">
         <v>230</v>
       </c>
       <c r="I12" t="s">
@@ -3554,28 +3567,28 @@
       </c>
     </row>
     <row r="13" ht="259.2" spans="1:9">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="8" t="s">
         <v>236</v>
       </c>
       <c r="I13" t="s">
@@ -3583,28 +3596,28 @@
       </c>
     </row>
     <row r="14" ht="129.6" spans="1:9">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="8" t="s">
         <v>242</v>
       </c>
       <c r="I14" t="s">
@@ -3612,28 +3625,28 @@
       </c>
     </row>
     <row r="15" ht="194.4" spans="1:9">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="8" t="s">
         <v>248</v>
       </c>
       <c r="I15" t="s">
@@ -3641,28 +3654,28 @@
       </c>
     </row>
     <row r="16" ht="226.8" spans="1:9">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="8" t="s">
         <v>255</v>
       </c>
       <c r="I16" t="s">
@@ -3670,28 +3683,28 @@
       </c>
     </row>
     <row r="17" ht="194.4" spans="1:9">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="8" t="s">
         <v>261</v>
       </c>
       <c r="I17" t="s">
@@ -3764,7 +3777,7 @@
       <c r="A2" t="s">
         <v>262</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>263</v>
       </c>
     </row>
@@ -3785,7 +3798,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C15" sqref="G7 C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
@@ -3828,39 +3841,53 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" ht="72" spans="1:7">
-      <c r="A2" t="s">
+    <row r="2" ht="81" spans="1:8">
+      <c r="A2" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="3" ht="57.6" spans="2:5">
-      <c r="B3" s="3" t="s">
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" ht="81" spans="1:8">
+      <c r="A3" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>271</v>
-      </c>
+      <c r="E3" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="H3" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Verify "Add to Wishlist" functionality with login
</commit_message>
<xml_diff>
--- a/Test Data/ECT-TestCases.xlsx
+++ b/Test Data/ECT-TestCases.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="315">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -1902,7 +1902,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1919,12 +1919,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2548,10 +2542,10 @@
       <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="5" t="s">
@@ -2560,7 +2554,7 @@
       <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2577,10 +2571,10 @@
       <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G3" s="5" t="s">
@@ -2589,7 +2583,7 @@
       <c r="H3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2609,7 +2603,7 @@
       <c r="E4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="10" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -2618,7 +2612,7 @@
       <c r="H4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2638,7 +2632,7 @@
       <c r="E5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="10" t="s">
         <v>36</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -2647,7 +2641,7 @@
       <c r="H5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2673,7 +2667,7 @@
       <c r="H6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2699,7 +2693,7 @@
       <c r="H7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2725,7 +2719,7 @@
       <c r="H8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2799,10 +2793,10 @@
       <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>63</v>
       </c>
       <c r="G2" s="5" t="s">
@@ -2811,7 +2805,7 @@
       <c r="H2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="11" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2828,7 +2822,7 @@
       <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>70</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -2840,7 +2834,7 @@
       <c r="H3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="12" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2857,7 +2851,7 @@
       <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="9" t="s">
         <v>78</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -2869,7 +2863,7 @@
       <c r="H4" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2898,7 +2892,7 @@
       <c r="H5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2915,7 +2909,7 @@
       <c r="D6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="9" t="s">
         <v>88</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -2924,7 +2918,7 @@
       <c r="G6" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2953,7 +2947,7 @@
       <c r="H7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2973,7 +2967,7 @@
       <c r="E8" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="8" t="s">
         <v>101</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -2982,7 +2976,7 @@
       <c r="H8" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3008,7 +3002,7 @@
       <c r="H9" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3025,10 +3019,10 @@
       <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="10" t="s">
         <v>114</v>
       </c>
       <c r="G10" s="5" t="s">
@@ -3037,7 +3031,7 @@
       <c r="H10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="13" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3054,7 +3048,7 @@
       <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="9" t="s">
         <v>118</v>
       </c>
       <c r="F11" s="4" t="s">
@@ -3086,7 +3080,7 @@
       <c r="E12" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="8" t="s">
         <v>101</v>
       </c>
       <c r="G12" s="4" t="s">
@@ -3112,7 +3106,7 @@
       <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="9" t="s">
         <v>130</v>
       </c>
       <c r="F13" s="4" t="s">
@@ -3207,7 +3201,7 @@
       <c r="E2" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>101</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -3353,7 +3347,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView topLeftCell="C15" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -3423,7 +3417,7 @@
       <c r="H2" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3928,7 +3922,7 @@
       <c r="A2" t="s">
         <v>262</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>263</v>
       </c>
     </row>
@@ -3949,7 +3943,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -4008,11 +4002,11 @@
       <c r="E2" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="3"/>
       <c r="G2" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" ht="64.8" spans="1:8">
       <c r="A3" s="3" t="s">
@@ -4030,99 +4024,99 @@
       <c r="E3" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" ht="81" spans="1:8">
       <c r="A4" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>276</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" ht="97.2" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>281</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7" t="s">
+      <c r="F5" s="3"/>
+      <c r="G5" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" ht="97.2" spans="1:8">
       <c r="A6" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="4" t="s">
         <v>286</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7" t="s">
+      <c r="F6" s="3"/>
+      <c r="G6" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="H6" s="6"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" ht="97.2" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>291</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7" t="s">
+      <c r="F7" s="3"/>
+      <c r="G7" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" ht="81" spans="1:7">
       <c r="A8" s="3" t="s">
@@ -4137,7 +4131,7 @@
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="4" t="s">
         <v>297</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -4148,67 +4142,69 @@
       <c r="A9" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="4" t="s">
         <v>301</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7" t="s">
+      <c r="F9" s="3"/>
+      <c r="G9" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" ht="145.8" spans="1:8">
       <c r="A10" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="4" t="s">
         <v>306</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7" t="s">
+      <c r="F10" s="3"/>
+      <c r="G10" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" ht="97.2" spans="1:8">
       <c r="A11" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="4" t="s">
         <v>311</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7" t="s">
+      <c r="F11" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" ht="16.2" spans="1:1">
       <c r="A12" s="3" t="s">

</xml_diff>